<commit_message>
Everything works except the staff view member
</commit_message>
<xml_diff>
--- a/data/attendance.xlsx
+++ b/data/attendance.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -685,6 +685,56 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-03-13</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>4</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Amna</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>01:05:56</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>01:06:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-03-13</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>3</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>nabeel</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>01:18:49</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>01:18:55</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
package page set properly
</commit_message>
<xml_diff>
--- a/data/attendance.xlsx
+++ b/data/attendance.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -735,6 +735,56 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-03-17</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>4</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Amna</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>01:47:07</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>01:47:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-03-17</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>nabeel</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>01:47:13</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>01:47:20</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Just the report page is left for setting
</commit_message>
<xml_diff>
--- a/data/attendance.xlsx
+++ b/data/attendance.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,6 +460,73 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2025-03-23</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1001</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Saboor Usman</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>07:22:07</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>07:29:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-03-23</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1002</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>qasim</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>07:22:21</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-03-23</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1005</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>hassaan</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>07:22:57</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
deleted the dummy data
</commit_message>
<xml_diff>
--- a/data/attendance.xlsx
+++ b/data/attendance.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hassaan\Documents\everything\project\New folder\gym_management\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962422BF-F09F-44FE-8D85-D5F314312AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>date</t>
   </si>
@@ -30,60 +36,12 @@
   <si>
     <t>check_out</t>
   </si>
-  <si>
-    <t>2025-03-23</t>
-  </si>
-  <si>
-    <t>1006</t>
-  </si>
-  <si>
-    <t>Saboor Usman</t>
-  </si>
-  <si>
-    <t>qasim</t>
-  </si>
-  <si>
-    <t>hassaan</t>
-  </si>
-  <si>
-    <t>bisma</t>
-  </si>
-  <si>
-    <t>Abdullah</t>
-  </si>
-  <si>
-    <t>07:22:07</t>
-  </si>
-  <si>
-    <t>07:22:21</t>
-  </si>
-  <si>
-    <t>07:22:57</t>
-  </si>
-  <si>
-    <t>07:37:36</t>
-  </si>
-  <si>
-    <t>11:39:42</t>
-  </si>
-  <si>
-    <t>07:29:18</t>
-  </si>
-  <si>
-    <t>07:59:48</t>
-  </si>
-  <si>
-    <t>11:36:03</t>
-  </si>
-  <si>
-    <t>11:36:11</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,13 +104,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -190,7 +156,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -224,6 +190,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -258,9 +225,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -433,14 +401,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="A2:E6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -457,88 +427,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>1001</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>1002</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>1005</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>1003</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>